<commit_message>
Working on Visualizations for Oct meeting.
</commit_message>
<xml_diff>
--- a/Data/export.xlsx
+++ b/Data/export.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Projects\FoodHubs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\FoodHubs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71092D7E-CD6A-4555-9322-FBD94F9A7267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19ABC86-30D1-4827-9C9E-9D0681695DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
   </bookViews>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1094">
   <si>
     <t>Decision Making</t>
   </si>
@@ -3393,6 +3393,9 @@
   </si>
   <si>
     <t>variety</t>
+  </si>
+  <si>
+    <t>specialized</t>
   </si>
   <si>
     <t>Specialized: Mainly focused on one or a very small set of items</t>
@@ -13895,8 +13898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4E1B48-BE1D-455E-923F-71BF6A05F081}">
   <dimension ref="A1:AW36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -13944,7 +13947,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="57" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -13993,13 +13996,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>14</v>
@@ -14041,7 +14044,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="41" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="U2" s="42" t="s">
         <v>28</v>
@@ -14074,34 +14077,34 @@
         <v>36</v>
       </c>
       <c r="AE2" s="44" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="AF2" s="44" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="AG2" s="44" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="AH2" s="41" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="AI2" s="41" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="AJ2" s="41" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="AK2" s="54" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="AL2" s="41" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="AM2" s="41" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="AN2" s="41" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="AO2" s="77" t="s">
         <v>43</v>
@@ -14113,7 +14116,7 @@
         <v>45</v>
       </c>
       <c r="AR2" s="40" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="3" spans="1:49">
@@ -14127,7 +14130,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>49</v>
@@ -14393,11 +14396,11 @@
         <v>0.2</v>
       </c>
       <c r="AR4" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="AS4" s="94"/>
       <c r="AT4" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="AU4">
         <v>127.5</v>
@@ -14481,7 +14484,7 @@
         <v>0.4</v>
       </c>
       <c r="W5" s="57" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="X5" s="53">
         <v>0</v>
@@ -14546,11 +14549,11 @@
         <v>0</v>
       </c>
       <c r="AR5" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="AS5" s="76"/>
       <c r="AT5" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="AU5">
         <v>255</v>
@@ -14699,11 +14702,11 @@
         <v>0.1</v>
       </c>
       <c r="AR6" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="AS6" s="95"/>
       <c r="AT6" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="AU6">
         <v>114.75</v>
@@ -14726,7 +14729,7 @@
         <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E7" s="51">
         <v>1</v>
@@ -14852,11 +14855,11 @@
         <v>0</v>
       </c>
       <c r="AR7" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="AS7" s="76"/>
       <c r="AT7" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="AU7">
         <v>255</v>
@@ -14879,7 +14882,7 @@
         <v>66</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E8" s="48">
         <v>1</v>
@@ -15003,11 +15006,11 @@
         <v>0.9</v>
       </c>
       <c r="AR8" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="AS8" s="80"/>
       <c r="AT8" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="AU8">
         <v>25.5</v>
@@ -15091,7 +15094,7 @@
         <v>0.4</v>
       </c>
       <c r="W9" s="57" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="X9" s="53">
         <v>80</v>
@@ -15156,11 +15159,11 @@
         <v>0</v>
       </c>
       <c r="AR9" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="AS9" s="96"/>
       <c r="AT9" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="AU9">
         <v>229.5</v>
@@ -15309,11 +15312,11 @@
         <v>0</v>
       </c>
       <c r="AR10" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="AS10" s="97"/>
       <c r="AT10" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="AU10">
         <v>127.5</v>
@@ -15336,7 +15339,7 @@
         <v>48</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E11" s="48">
         <v>0</v>
@@ -15397,7 +15400,7 @@
         <v>0</v>
       </c>
       <c r="W11" s="59" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
       <c r="X11" s="60">
         <v>34</v>
@@ -15460,11 +15463,11 @@
         <v>0.45</v>
       </c>
       <c r="AR11" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="AS11" s="98"/>
       <c r="AT11" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="AU11">
         <v>25.5</v>
@@ -15613,11 +15616,11 @@
         <v>0.5</v>
       </c>
       <c r="AR12" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="AS12" s="84"/>
       <c r="AT12" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="AU12">
         <v>127.5</v>
@@ -15701,7 +15704,7 @@
         <v>0.4</v>
       </c>
       <c r="W13" s="57" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="X13" s="53">
         <v>0</v>
@@ -15766,11 +15769,11 @@
         <v>0.5</v>
       </c>
       <c r="AR13" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="AS13" s="99"/>
       <c r="AT13" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="AU13">
         <v>0</v>
@@ -15793,7 +15796,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E14" s="48">
         <v>0</v>
@@ -15917,11 +15920,11 @@
         <v>0.05</v>
       </c>
       <c r="AR14" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="AS14" s="100"/>
       <c r="AT14" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="AU14">
         <v>127.5</v>
@@ -15982,7 +15985,7 @@
       <c r="AK16" s="53"/>
       <c r="AO16" s="53"/>
       <c r="AS16" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="17" spans="1:43">
@@ -16109,7 +16112,7 @@
       <c r="N23" s="102"/>
       <c r="O23" s="102"/>
       <c r="P23" s="103" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="Q23" s="104"/>
       <c r="R23" s="104"/>
@@ -16118,7 +16121,7 @@
       <c r="U23" s="104"/>
       <c r="V23" s="105"/>
       <c r="W23" s="106" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="AB23" s="101" t="s">
         <v>99</v>
@@ -29776,32 +29779,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0B965-A240-4E89-B3BD-8E511D00AD0F}">
-  <dimension ref="A1:AR13"/>
+  <dimension ref="A1:AQ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:43">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1" t="s">
         <v>1092</v>
       </c>
-      <c r="C1" t="s">
-        <v>1091</v>
-      </c>
       <c r="D1" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="G1" t="s">
         <v>14</v>
@@ -29810,115 +29813,106 @@
         <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>1080</v>
       </c>
       <c r="R1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="T1" t="s">
-        <v>1079</v>
+        <v>4</v>
       </c>
       <c r="U1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="X1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Y1" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="AA1" t="s">
-        <v>33</v>
+        <v>269</v>
       </c>
       <c r="AB1" t="s">
-        <v>34</v>
+        <v>1081</v>
       </c>
       <c r="AC1" t="s">
-        <v>35</v>
+        <v>1082</v>
       </c>
       <c r="AD1" t="s">
-        <v>36</v>
+        <v>1083</v>
       </c>
       <c r="AE1" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="AF1" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="AG1" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="AH1" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="AI1" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c r="AJ1" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c r="AK1" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
       <c r="AL1" t="s">
-        <v>1087</v>
+        <v>43</v>
       </c>
       <c r="AM1" t="s">
-        <v>1088</v>
+        <v>44</v>
       </c>
       <c r="AN1" t="s">
-        <v>1089</v>
+        <v>45</v>
       </c>
       <c r="AO1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -29929,7 +29923,7 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E2" t="s">
         <v>49</v>
@@ -29943,116 +29937,107 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>49</v>
       </c>
-      <c r="J2" t="s">
+      <c r="U2">
+        <v>100</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" t="s">
         <v>49</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Z2" t="s">
         <v>49</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>49</v>
       </c>
-      <c r="X2">
-        <v>100</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>49</v>
+      <c r="AB2">
+        <v>3</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
       </c>
       <c r="AE2">
         <v>3</v>
       </c>
       <c r="AF2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH2">
-        <v>3</v>
+        <v>177.06984362075525</v>
       </c>
       <c r="AI2">
-        <v>2</v>
+        <v>502.86279698478472</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>110.02609983990698</v>
       </c>
       <c r="AK2">
-        <v>177.06984362075525</v>
+        <v>312.46445569423616</v>
       </c>
       <c r="AL2">
-        <v>502.86279698478472</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>110.02609983990698</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>312.46445569423616</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -30078,115 +30063,109 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0.5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>0.6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3">
+        <v>90</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3">
+        <v>2.6</v>
+      </c>
+      <c r="Z3">
+        <v>2.75</v>
+      </c>
+      <c r="AA3">
+        <v>2.5</v>
+      </c>
+      <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+      <c r="AD3">
         <v>2</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0.5</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>0.6</v>
-      </c>
-      <c r="W3" t="s">
-        <v>1056</v>
-      </c>
-      <c r="X3">
-        <v>10</v>
-      </c>
-      <c r="Y3">
-        <v>90</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB3">
-        <v>2.6</v>
-      </c>
-      <c r="AC3">
-        <v>2.75</v>
-      </c>
-      <c r="AD3">
-        <v>2.5</v>
       </c>
       <c r="AE3">
         <v>3</v>
       </c>
       <c r="AF3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH3">
-        <v>3</v>
+        <v>66.730648916437048</v>
       </c>
       <c r="AI3">
-        <v>2</v>
+        <v>180.79488361545049</v>
       </c>
       <c r="AJ3">
-        <v>1</v>
+        <v>41.464502875977445</v>
       </c>
       <c r="AK3">
-        <v>66.730648916437048</v>
+        <v>112.34073238254251</v>
       </c>
       <c r="AL3">
-        <v>180.79488361545049</v>
+        <v>0.5</v>
       </c>
       <c r="AM3">
-        <v>41.464502875977445</v>
+        <v>0.3</v>
       </c>
       <c r="AN3">
-        <v>112.34073238254251</v>
-      </c>
-      <c r="AO3">
-        <v>0.5</v>
-      </c>
-      <c r="AP3">
-        <v>0.3</v>
-      </c>
-      <c r="AQ3">
         <v>0.2</v>
       </c>
-      <c r="AR3" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44">
+      <c r="AO3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -30212,115 +30191,109 @@
         <v>1</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
       <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1065</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>100</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4">
+        <v>2.8</v>
+      </c>
+      <c r="Z4">
+        <v>2.5</v>
+      </c>
+      <c r="AA4">
+        <v>2.5</v>
+      </c>
+      <c r="AB4">
         <v>2</v>
       </c>
-      <c r="V4">
-        <v>0.4</v>
-      </c>
-      <c r="W4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>100</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB4">
-        <v>2.8</v>
-      </c>
       <c r="AC4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AD4">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AE4">
         <v>2</v>
       </c>
       <c r="AF4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG4">
         <v>3</v>
       </c>
       <c r="AH4">
-        <v>2</v>
+        <v>54.000686345069504</v>
       </c>
       <c r="AI4">
-        <v>1</v>
+        <v>107.42790056424694</v>
       </c>
       <c r="AJ4">
-        <v>3</v>
+        <v>33.554470855870157</v>
       </c>
       <c r="AK4">
-        <v>54.000686345069504</v>
+        <v>66.752602653159883</v>
       </c>
       <c r="AL4">
-        <v>107.42790056424694</v>
+        <v>1</v>
       </c>
       <c r="AM4">
-        <v>33.554470855870157</v>
+        <v>0</v>
       </c>
       <c r="AN4">
-        <v>66.752602653159883</v>
-      </c>
-      <c r="AO4">
-        <v>1</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -30346,115 +30319,109 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="U5">
+        <v>33</v>
+      </c>
+      <c r="V5">
+        <v>64</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y5">
         <v>2</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0.5</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X5">
-        <v>33</v>
-      </c>
-      <c r="Y5">
-        <v>64</v>
-      </c>
       <c r="Z5">
-        <v>3</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>63</v>
+        <v>1.25</v>
+      </c>
+      <c r="AA5">
+        <v>1.5</v>
       </c>
       <c r="AB5">
         <v>2</v>
       </c>
       <c r="AC5">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="AD5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AE5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF5">
         <v>2</v>
       </c>
       <c r="AG5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH5">
-        <v>3</v>
+        <v>59.07183056002777</v>
       </c>
       <c r="AI5">
-        <v>2</v>
+        <v>62.670818674705536</v>
       </c>
       <c r="AJ5">
-        <v>1</v>
+        <v>36.705533782726235</v>
       </c>
       <c r="AK5">
-        <v>59.07183056002777</v>
+        <v>38.941841318391553</v>
       </c>
       <c r="AL5">
-        <v>62.670818674705536</v>
+        <v>0.45</v>
       </c>
       <c r="AM5">
-        <v>36.705533782726235</v>
+        <v>0.45</v>
       </c>
       <c r="AN5">
-        <v>38.941841318391553</v>
-      </c>
-      <c r="AO5">
-        <v>0.45</v>
-      </c>
-      <c r="AP5">
-        <v>0.45</v>
-      </c>
-      <c r="AQ5">
         <v>0.1</v>
       </c>
-      <c r="AR5" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44">
+      <c r="AO5" t="s">
+        <v>1069</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -30465,7 +30432,7 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -30480,73 +30447,73 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0.2</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="U6">
+        <v>80</v>
+      </c>
+      <c r="V6">
+        <v>20</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6">
+        <v>2.8</v>
+      </c>
+      <c r="Z6">
+        <v>3</v>
+      </c>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
         <v>2</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0.5</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
-      <c r="V6">
-        <v>0.2</v>
-      </c>
-      <c r="W6" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X6">
-        <v>80</v>
-      </c>
-      <c r="Y6">
-        <v>20</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB6">
-        <v>2.8</v>
-      </c>
       <c r="AC6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD6">
         <v>3</v>
       </c>
       <c r="AE6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <v>2</v>
@@ -30555,40 +30522,34 @@
         <v>3</v>
       </c>
       <c r="AH6">
-        <v>1</v>
+        <v>61.132335382406808</v>
       </c>
       <c r="AI6">
-        <v>2</v>
+        <v>510.85624675116685</v>
       </c>
       <c r="AJ6">
-        <v>3</v>
+        <v>37.985872120818676</v>
       </c>
       <c r="AK6">
-        <v>61.132335382406808</v>
+        <v>317.43135510566225</v>
       </c>
       <c r="AL6">
-        <v>510.85624675116685</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>37.985872120818676</v>
+        <v>0</v>
       </c>
       <c r="AN6">
-        <v>317.43135510566225</v>
-      </c>
-      <c r="AO6">
-        <v>1</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -30599,7 +30560,7 @@
         <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -30614,14 +30575,14 @@
         <v>0</v>
       </c>
       <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
       <c r="L7">
         <v>1</v>
       </c>
@@ -30629,7 +30590,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -30638,91 +30599,85 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1055</v>
       </c>
       <c r="U7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>0.8</v>
-      </c>
-      <c r="W7" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>49</v>
       </c>
       <c r="AA7" t="s">
         <v>49</v>
       </c>
-      <c r="AB7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>49</v>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>2</v>
+      </c>
+      <c r="AD7">
+        <v>3</v>
       </c>
       <c r="AE7">
         <v>2</v>
       </c>
       <c r="AF7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <v>3</v>
       </c>
-      <c r="AH7">
-        <v>2</v>
-      </c>
-      <c r="AI7">
-        <v>1</v>
-      </c>
-      <c r="AJ7">
-        <v>3</v>
+      <c r="AH7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>49</v>
       </c>
       <c r="AK7" t="s">
         <v>49</v>
       </c>
-      <c r="AL7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO7">
+      <c r="AL7">
         <v>0.1</v>
       </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7">
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
         <v>0.9</v>
       </c>
-      <c r="AR7" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44">
+      <c r="AO7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -30754,64 +30709,64 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1065</v>
       </c>
       <c r="U8">
+        <v>80</v>
+      </c>
+      <c r="V8">
+        <v>15</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y8">
+        <v>2.8</v>
+      </c>
+      <c r="Z8">
+        <v>2.25</v>
+      </c>
+      <c r="AA8">
+        <v>1.5</v>
+      </c>
+      <c r="AB8">
         <v>2</v>
       </c>
-      <c r="V8">
-        <v>0.4</v>
-      </c>
-      <c r="W8" t="s">
-        <v>1064</v>
-      </c>
-      <c r="X8">
-        <v>80</v>
-      </c>
-      <c r="Y8">
-        <v>15</v>
-      </c>
-      <c r="Z8">
-        <v>5</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB8">
-        <v>2.8</v>
-      </c>
       <c r="AC8">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AE8">
         <v>2</v>
@@ -30823,40 +30778,34 @@
         <v>3</v>
       </c>
       <c r="AH8">
-        <v>2</v>
+        <v>42.020373634883299</v>
       </c>
       <c r="AI8">
-        <v>1</v>
+        <v>244.99066061451242</v>
       </c>
       <c r="AJ8">
-        <v>3</v>
+        <v>26.110249663765671</v>
       </c>
       <c r="AK8">
-        <v>42.020373634883299</v>
+        <v>152.23013887305163</v>
       </c>
       <c r="AL8">
-        <v>244.99066061451242</v>
+        <v>0.9</v>
       </c>
       <c r="AM8">
-        <v>26.110249663765671</v>
+        <v>0.1</v>
       </c>
       <c r="AN8">
-        <v>152.23013887305163</v>
-      </c>
-      <c r="AO8">
-        <v>0.9</v>
-      </c>
-      <c r="AP8">
-        <v>0.1</v>
-      </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="9" spans="1:44">
+        <v>0</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>1070</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -30882,115 +30831,109 @@
         <v>1</v>
       </c>
       <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0.5</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="U9">
+        <v>90</v>
+      </c>
+      <c r="V9">
+        <v>10</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9">
+        <v>2.6</v>
+      </c>
+      <c r="Z9">
         <v>2</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0.5</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>5</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X9">
-        <v>90</v>
-      </c>
-      <c r="Y9">
-        <v>10</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>50</v>
+      <c r="AA9">
+        <v>2</v>
       </c>
       <c r="AB9">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9">
+        <v>3</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
         <v>2</v>
-      </c>
-      <c r="AD9">
-        <v>2</v>
-      </c>
-      <c r="AE9">
-        <v>2.5</v>
-      </c>
-      <c r="AF9">
-        <v>3</v>
       </c>
       <c r="AG9">
         <v>3</v>
       </c>
       <c r="AH9">
-        <v>1</v>
+        <v>69.284801167278431</v>
       </c>
       <c r="AI9">
-        <v>2</v>
+        <v>217.13337565699663</v>
       </c>
       <c r="AJ9">
-        <v>3</v>
+        <v>43.051579505238429</v>
       </c>
       <c r="AK9">
-        <v>69.284801167278431</v>
+        <v>134.9204245065049</v>
       </c>
       <c r="AL9">
-        <v>217.13337565699663</v>
+        <v>0.5</v>
       </c>
       <c r="AM9">
-        <v>43.051579505238429</v>
+        <v>0.5</v>
       </c>
       <c r="AN9">
-        <v>134.9204245065049</v>
-      </c>
-      <c r="AO9">
-        <v>0.5</v>
-      </c>
-      <c r="AP9">
-        <v>0.5</v>
-      </c>
-      <c r="AQ9">
-        <v>0</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -31001,7 +30944,7 @@
         <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -31016,7 +30959,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -31048,83 +30991,77 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10">
-        <v>0</v>
+      <c r="T10" t="s">
+        <v>1057</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10" t="s">
-        <v>1064</v>
-      </c>
-      <c r="X10">
-        <v>34</v>
-      </c>
-      <c r="Y10">
         <v>33</v>
       </c>
-      <c r="Z10">
+      <c r="W10">
         <v>33</v>
       </c>
+      <c r="X10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>49</v>
+      </c>
       <c r="AA10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB10" t="s">
         <v>49</v>
       </c>
-      <c r="AC10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>49</v>
+      <c r="AB10">
+        <v>3</v>
+      </c>
+      <c r="AC10">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <v>2</v>
       </c>
       <c r="AE10">
         <v>3</v>
       </c>
       <c r="AF10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG10">
-        <v>2</v>
-      </c>
-      <c r="AH10">
-        <v>3</v>
-      </c>
-      <c r="AI10">
-        <v>2</v>
-      </c>
-      <c r="AJ10">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>49</v>
       </c>
       <c r="AK10" t="s">
         <v>49</v>
       </c>
-      <c r="AL10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO10">
+      <c r="AL10">
         <v>0.1</v>
       </c>
-      <c r="AP10">
+      <c r="AM10">
         <v>0.45</v>
       </c>
-      <c r="AQ10">
+      <c r="AN10">
         <v>0.45</v>
       </c>
-      <c r="AR10" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44">
+      <c r="AO10" t="s">
+        <v>1073</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -31150,115 +31087,109 @@
         <v>0</v>
       </c>
       <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0.5</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>0.8</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1055</v>
+      </c>
+      <c r="U11">
+        <v>25</v>
+      </c>
+      <c r="V11">
+        <v>47</v>
+      </c>
+      <c r="W11">
+        <v>28</v>
+      </c>
+      <c r="X11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y11">
+        <v>2.6</v>
+      </c>
+      <c r="Z11">
+        <v>2.75</v>
+      </c>
+      <c r="AA11">
         <v>2</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>0.5</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>4</v>
-      </c>
-      <c r="V11">
-        <v>0.8</v>
-      </c>
-      <c r="W11" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X11">
-        <v>25</v>
-      </c>
-      <c r="Y11">
-        <v>47</v>
-      </c>
-      <c r="Z11">
-        <v>28</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>77</v>
-      </c>
       <c r="AB11">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="AC11">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="AD11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE11">
         <v>2</v>
       </c>
       <c r="AF11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG11">
         <v>3</v>
       </c>
       <c r="AH11">
-        <v>2</v>
+        <v>49.269501231495838</v>
       </c>
       <c r="AI11">
-        <v>1</v>
+        <v>219.39060746351947</v>
       </c>
       <c r="AJ11">
-        <v>3</v>
+        <v>30.614648721153365</v>
       </c>
       <c r="AK11">
-        <v>49.269501231495838</v>
+        <v>136.32300332528004</v>
       </c>
       <c r="AL11">
-        <v>219.39060746351947</v>
+        <v>0.5</v>
       </c>
       <c r="AM11">
-        <v>30.614648721153365</v>
+        <v>0</v>
       </c>
       <c r="AN11">
-        <v>136.32300332528004</v>
-      </c>
-      <c r="AO11">
         <v>0.5</v>
       </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11">
-        <v>0.5</v>
-      </c>
-      <c r="AR11" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44">
+      <c r="AO11" t="s">
+        <v>1074</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -31284,7 +31215,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -31296,103 +31227,97 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1065</v>
       </c>
       <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>10</v>
+      </c>
+      <c r="W12">
+        <v>90</v>
+      </c>
+      <c r="X12" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB12">
         <v>2</v>
       </c>
-      <c r="V12">
-        <v>0.4</v>
-      </c>
-      <c r="W12" t="s">
-        <v>1064</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>10</v>
-      </c>
-      <c r="Z12">
-        <v>90</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>49</v>
+      <c r="AC12">
+        <v>2</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
       </c>
       <c r="AE12">
         <v>2</v>
       </c>
       <c r="AF12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG12">
         <v>3</v>
       </c>
       <c r="AH12">
-        <v>2</v>
+        <v>102.89933989204253</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>195.67903527505888</v>
       </c>
       <c r="AJ12">
-        <v>3</v>
+        <v>63.938685509153132</v>
       </c>
       <c r="AK12">
-        <v>102.89933989204253</v>
+        <v>121.58931544471467</v>
       </c>
       <c r="AL12">
-        <v>195.67903527505888</v>
+        <v>0</v>
       </c>
       <c r="AM12">
-        <v>63.938685509153132</v>
+        <v>0.5</v>
       </c>
       <c r="AN12">
-        <v>121.58931544471467</v>
-      </c>
-      <c r="AO12">
-        <v>0</v>
-      </c>
-      <c r="AP12">
         <v>0.5</v>
       </c>
-      <c r="AQ12">
-        <v>0.5</v>
-      </c>
-      <c r="AR12" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="13" spans="1:44">
+      <c r="AO12" t="s">
+        <v>1075</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -31403,7 +31328,7 @@
         <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -31424,106 +31349,100 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1056</v>
       </c>
       <c r="U13">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="V13">
-        <v>0.6</v>
-      </c>
-      <c r="W13" t="s">
-        <v>1056</v>
-      </c>
-      <c r="X13">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>50</v>
       </c>
       <c r="Y13">
-        <v>20</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>50</v>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="AA13">
+        <v>1.5</v>
       </c>
       <c r="AB13">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="AC13">
-        <v>2.6666666666666665</v>
+        <v>2</v>
       </c>
       <c r="AD13">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AE13">
         <v>2</v>
       </c>
       <c r="AF13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG13">
-        <v>2</v>
-      </c>
-      <c r="AH13">
-        <v>2</v>
-      </c>
-      <c r="AI13">
-        <v>1</v>
-      </c>
-      <c r="AJ13">
         <v>3</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>49</v>
       </c>
       <c r="AK13" t="s">
         <v>49</v>
       </c>
-      <c r="AL13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO13">
+      <c r="AL13">
         <v>0.5</v>
       </c>
-      <c r="AP13">
+      <c r="AM13">
         <v>0.45</v>
       </c>
-      <c r="AQ13">
+      <c r="AN13">
         <v>0.05</v>
       </c>
-      <c r="AR13" t="s">
-        <v>1075</v>
+      <c r="AO13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>1076</v>
       </c>
     </row>
   </sheetData>
@@ -33993,7 +33912,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="M2" t="s">
         <v>282</v>
@@ -34778,7 +34697,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E1" sqref="E1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -34849,7 +34768,7 @@
         <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -34917,7 +34836,7 @@
         <v>208</v>
       </c>
       <c r="E8" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -34951,7 +34870,7 @@
         <v>229</v>
       </c>
       <c r="E10" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -34985,7 +34904,7 @@
         <v>244</v>
       </c>
       <c r="E12" t="s">
-        <v>1064</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -35007,17 +34926,17 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>